<commit_message>
Refactored code and Added manual test cases sheet.
</commit_message>
<xml_diff>
--- a/testData/Data.xlsx
+++ b/testData/Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankit\eclipse-workspace\qa-interview\Lampenwelt_UI\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankit\eclipse-workspace\Lampenwelt_UI\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35142C44-7466-4657-A30A-189348542BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CDB4FB-ECB5-41E8-9EEE-7E986794ABDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-15800" yWindow="70" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25710" yWindow="-3770" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -371,7 +371,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>